<commit_message>
Updates X for Y project with Fortran results
</commit_message>
<xml_diff>
--- a/published/x_for_y_devs/X_for_Y.xlsx
+++ b/published/x_for_y_devs/X_for_Y.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21105"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="1560" windowWidth="27440" windowHeight="18340" tabRatio="500"/>
+    <workbookView xWindow="680" yWindow="1180" windowWidth="27460" windowHeight="18340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$C$3:$N$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$C$3:$O$15</definedName>
     <definedName name="x_for_y_devs" localSheetId="0">Sheet1!#REF!</definedName>
     <definedName name="x_for_y_devs" localSheetId="1">'Sheet1 (2)'!#REF!</definedName>
-    <definedName name="x_for_y_devs_1" localSheetId="0">Sheet1!$D$4:$N$14</definedName>
+    <definedName name="x_for_y_devs_1" localSheetId="0">Sheet1!$D$4:$O$15</definedName>
     <definedName name="x_for_y_devs_1" localSheetId="1">'Sheet1 (2)'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -29,7 +29,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="x_for_y_devs.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:pberkes:o:x_for_y_devs:x_for_y_devs.csv" space="1" consecutive="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:pberkes:o:x_for_y_devs:x_for_y_devs.csv" space="1" consecutive="1">
       <textFields count="12">
         <textField type="skip"/>
         <textField/>
@@ -47,7 +47,7 @@
     </textPr>
   </connection>
   <connection id="2" name="x_for_y_devs.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:pberkes:o:x_for_y_devs:x_for_y_devs.csv" delimited="0" space="1" consecutive="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:pberkes:o:x_for_y_devs:x_for_y_devs.csv" delimited="0" space="1" consecutive="1">
       <textFields count="11">
         <textField type="text"/>
         <textField position="13"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
   <si>
     <t>BASIC</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>X for Y developers</t>
+  </si>
+  <si>
+    <t>Fortran</t>
   </si>
 </sst>
 </file>
@@ -403,10 +406,6 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -440,6 +439,10 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -498,7 +501,18 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -829,50 +843,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:N14"/>
+  <dimension ref="D1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:N14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="3" width="9.5" style="3" customWidth="1"/>
-    <col min="4" max="14" width="9.5" customWidth="1"/>
-    <col min="15" max="24" width="10.83203125" style="3"/>
-    <col min="25" max="25" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="10.83203125" style="3"/>
+    <col min="4" max="15" width="10" customWidth="1"/>
+    <col min="16" max="25" width="10.83203125" style="3"/>
+    <col min="26" max="26" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:14" ht="57" customHeight="1"/>
-    <row r="2" spans="4:14" ht="57" customHeight="1">
-      <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-    </row>
-    <row r="3" spans="4:14" ht="57" customHeight="1">
-      <c r="E3" s="4" t="s">
+    <row r="1" spans="4:15" ht="57" customHeight="1"/>
+    <row r="2" spans="4:15" ht="57" customHeight="1">
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+    </row>
+    <row r="3" spans="4:15" ht="57" customHeight="1">
+      <c r="E3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-    </row>
-    <row r="4" spans="4:14" ht="57" customHeight="1" thickBot="1">
-      <c r="D4" s="6" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+    </row>
+    <row r="4" spans="4:15" ht="60" customHeight="1" thickBot="1">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -888,437 +904,460 @@
         <v>3</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="4:14" ht="57" customHeight="1">
+    <row r="5" spans="4:15" ht="60" customHeight="1">
       <c r="D5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="6">
         <v>7</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>331</v>
       </c>
-      <c r="G5" s="9">
-        <v>0</v>
-      </c>
-      <c r="H5" s="9">
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
         <v>10502</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7">
         <v>12</v>
       </c>
-      <c r="J5" s="9">
-        <v>0</v>
-      </c>
-      <c r="K5" s="9">
-        <v>0</v>
-      </c>
-      <c r="L5" s="9">
-        <v>0</v>
-      </c>
-      <c r="M5" s="9">
-        <v>0</v>
-      </c>
-      <c r="N5" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="4:14" ht="57" customHeight="1">
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0</v>
+      </c>
+      <c r="N5" s="7">
+        <v>0</v>
+      </c>
+      <c r="O5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="4:15" ht="60" customHeight="1">
       <c r="D6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="9">
         <v>5</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <v>15140</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="10">
         <v>5260</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="10">
         <v>8</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="10">
+        <v>16900</v>
+      </c>
+      <c r="J6" s="10">
         <v>114900</v>
       </c>
-      <c r="J6" s="12">
-        <v>0</v>
-      </c>
-      <c r="K6" s="12">
-        <v>0</v>
-      </c>
-      <c r="L6" s="12">
+      <c r="K6" s="10">
+        <v>0</v>
+      </c>
+      <c r="L6" s="10">
+        <v>0</v>
+      </c>
+      <c r="M6" s="10">
         <v>7570</v>
       </c>
-      <c r="M6" s="12">
+      <c r="N6" s="10">
         <v>1830</v>
       </c>
-      <c r="N6" s="13">
+      <c r="O6" s="11">
         <v>2620</v>
       </c>
     </row>
-    <row r="7" spans="4:14" ht="57" customHeight="1">
+    <row r="7" spans="4:15" ht="60" customHeight="1">
       <c r="D7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="9">
         <v>2</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="10">
         <v>46000</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="10">
         <v>2200</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="10">
         <v>3</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="10">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
         <v>1357000</v>
       </c>
-      <c r="J7" s="12">
-        <v>0</v>
-      </c>
-      <c r="K7" s="12">
-        <v>0</v>
-      </c>
-      <c r="L7" s="12">
+      <c r="K7" s="10">
+        <v>0</v>
+      </c>
+      <c r="L7" s="10">
+        <v>0</v>
+      </c>
+      <c r="M7" s="10">
         <v>4</v>
       </c>
-      <c r="M7" s="12">
+      <c r="N7" s="10">
         <v>3</v>
       </c>
-      <c r="N7" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="4:14" ht="57" customHeight="1">
+      <c r="O7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="4:15" ht="60" customHeight="1">
       <c r="D8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="11">
-        <v>0</v>
-      </c>
-      <c r="F8" s="12">
-        <v>0</v>
-      </c>
-      <c r="G8" s="12">
-        <v>0</v>
-      </c>
-      <c r="H8" s="12">
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
         <v>7</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="10">
+        <v>0</v>
+      </c>
+      <c r="J8" s="10">
         <v>3</v>
       </c>
-      <c r="J8" s="12">
-        <v>0</v>
-      </c>
-      <c r="K8" s="12">
-        <v>0</v>
-      </c>
-      <c r="L8" s="12">
-        <v>0</v>
-      </c>
-      <c r="M8" s="12">
-        <v>0</v>
-      </c>
-      <c r="N8" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="4:14" ht="57" customHeight="1">
+      <c r="K8" s="10">
+        <v>0</v>
+      </c>
+      <c r="L8" s="10">
+        <v>0</v>
+      </c>
+      <c r="M8" s="10">
+        <v>0</v>
+      </c>
+      <c r="N8" s="10">
+        <v>0</v>
+      </c>
+      <c r="O8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="4:15" ht="60" customHeight="1">
       <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0</v>
+      </c>
+      <c r="I9" s="10">
         <v>4</v>
       </c>
-      <c r="E9" s="11">
+      <c r="J9" s="10">
+        <v>0</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0</v>
+      </c>
+      <c r="L9" s="10">
+        <v>0</v>
+      </c>
+      <c r="M9" s="10">
+        <v>0</v>
+      </c>
+      <c r="N9" s="10">
+        <v>0</v>
+      </c>
+      <c r="O9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="4:15" ht="60" customHeight="1">
+      <c r="D10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="9">
         <v>62</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F10" s="10">
         <v>21100</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G10" s="10">
         <v>4185</v>
       </c>
-      <c r="H9" s="12">
-        <v>537760</v>
-      </c>
-      <c r="I9" s="12">
+      <c r="H10" s="10">
+        <v>95213</v>
+      </c>
+      <c r="I10" s="10">
+        <v>8</v>
+      </c>
+      <c r="J10" s="10">
         <v>286200</v>
       </c>
-      <c r="J9" s="12">
-        <v>0</v>
-      </c>
-      <c r="K9" s="12">
+      <c r="K10" s="10">
+        <v>0</v>
+      </c>
+      <c r="L10" s="10">
         <v>55</v>
       </c>
-      <c r="L9" s="12">
+      <c r="M10" s="10">
         <v>10373</v>
       </c>
-      <c r="M9" s="12">
+      <c r="N10" s="10">
         <v>543</v>
       </c>
-      <c r="N9" s="13">
+      <c r="O10" s="11">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="4:14" ht="57" customHeight="1">
-      <c r="D10" s="3" t="s">
+    <row r="11" spans="4:15" ht="60" customHeight="1">
+      <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="11">
-        <v>0</v>
-      </c>
-      <c r="F10" s="12">
-        <v>0</v>
-      </c>
-      <c r="G10" s="12">
+      <c r="E11" s="9">
+        <v>0</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0</v>
+      </c>
+      <c r="G11" s="10">
         <v>13360</v>
       </c>
-      <c r="H10" s="12">
-        <v>0</v>
-      </c>
-      <c r="I10" s="12">
+      <c r="H11" s="10">
+        <v>0</v>
+      </c>
+      <c r="I11" s="10">
+        <v>7</v>
+      </c>
+      <c r="J11" s="10">
         <v>52500</v>
       </c>
-      <c r="J10" s="12">
+      <c r="K11" s="10">
         <v>5</v>
       </c>
-      <c r="K10" s="12">
-        <v>0</v>
-      </c>
-      <c r="L10" s="12">
+      <c r="L11" s="10">
+        <v>0</v>
+      </c>
+      <c r="M11" s="10">
         <v>14604</v>
       </c>
-      <c r="M10" s="12">
+      <c r="N11" s="10">
         <v>5</v>
       </c>
-      <c r="N10" s="13">
+      <c r="O11" s="11">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="4:14" ht="57" customHeight="1">
-      <c r="D11" s="3" t="s">
+    <row r="12" spans="4:15" ht="60" customHeight="1">
+      <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E12" s="9">
         <v>2</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F12" s="10">
         <v>7</v>
       </c>
-      <c r="G11" s="12">
-        <v>0</v>
-      </c>
-      <c r="H11" s="12">
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
         <v>3280</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I12" s="10">
+        <v>8</v>
+      </c>
+      <c r="J12" s="10">
         <v>1366</v>
       </c>
-      <c r="J11" s="12">
-        <v>0</v>
-      </c>
-      <c r="K11" s="12">
+      <c r="K12" s="10">
+        <v>0</v>
+      </c>
+      <c r="L12" s="10">
         <v>4400</v>
       </c>
-      <c r="L11" s="12">
+      <c r="M12" s="10">
         <v>7</v>
       </c>
-      <c r="M11" s="12">
+      <c r="N12" s="10">
         <v>1410</v>
       </c>
-      <c r="N11" s="13">
+      <c r="O12" s="11">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="4:14" ht="57" customHeight="1">
-      <c r="D12" s="3" t="s">
+    <row r="13" spans="4:15" ht="60" customHeight="1">
+      <c r="D13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E13" s="9">
         <v>7</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F13" s="10">
         <v>10910</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G13" s="10">
         <v>12</v>
       </c>
-      <c r="H12" s="12">
-        <v>0</v>
-      </c>
-      <c r="I12" s="12">
+      <c r="H13" s="10">
+        <v>0</v>
+      </c>
+      <c r="I13" s="10">
+        <v>11600</v>
+      </c>
+      <c r="J13" s="10">
         <v>16380</v>
       </c>
-      <c r="J12" s="12">
+      <c r="K13" s="10">
         <v>4203</v>
       </c>
-      <c r="K12" s="12">
+      <c r="L13" s="10">
         <v>22100</v>
       </c>
-      <c r="L12" s="12">
+      <c r="M13" s="10">
         <v>13</v>
       </c>
-      <c r="M12" s="12">
+      <c r="N13" s="10">
         <v>15600</v>
       </c>
-      <c r="N12" s="13">
+      <c r="O13" s="11">
         <v>1984</v>
       </c>
     </row>
-    <row r="13" spans="4:14" ht="57" customHeight="1">
-      <c r="D13" s="3" t="s">
+    <row r="14" spans="4:15" ht="60" customHeight="1">
+      <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="11">
-        <v>0</v>
-      </c>
-      <c r="F13" s="12">
+      <c r="E14" s="9">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10">
         <v>1650</v>
       </c>
-      <c r="G13" s="12">
-        <v>0</v>
-      </c>
-      <c r="H13" s="12">
-        <v>0</v>
-      </c>
-      <c r="I13" s="12">
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10">
+        <v>2</v>
+      </c>
+      <c r="J14" s="10">
         <v>1799</v>
       </c>
-      <c r="J13" s="12">
-        <v>0</v>
-      </c>
-      <c r="K13" s="12">
+      <c r="K14" s="10">
+        <v>0</v>
+      </c>
+      <c r="L14" s="10">
         <v>5</v>
       </c>
-      <c r="L13" s="12">
+      <c r="M14" s="10">
         <v>6</v>
       </c>
-      <c r="M13" s="12">
-        <v>0</v>
-      </c>
-      <c r="N13" s="13">
+      <c r="N14" s="10">
+        <v>0</v>
+      </c>
+      <c r="O14" s="11">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="4:14" ht="57" customHeight="1" thickBot="1">
-      <c r="D14" s="3" t="s">
+    <row r="15" spans="4:15" ht="60" customHeight="1" thickBot="1">
+      <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="15">
+      <c r="E15" s="12">
+        <v>0</v>
+      </c>
+      <c r="F15" s="13">
         <v>78</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G15" s="13">
         <v>2056</v>
       </c>
-      <c r="H14" s="15">
-        <v>0</v>
-      </c>
-      <c r="I14" s="15">
+      <c r="H15" s="13">
+        <v>0</v>
+      </c>
+      <c r="I15" s="13">
+        <v>0</v>
+      </c>
+      <c r="J15" s="13">
         <v>88120</v>
       </c>
-      <c r="J14" s="15">
-        <v>0</v>
-      </c>
-      <c r="K14" s="15">
-        <v>0</v>
-      </c>
-      <c r="L14" s="15">
+      <c r="K15" s="13">
+        <v>0</v>
+      </c>
+      <c r="L15" s="13">
+        <v>0</v>
+      </c>
+      <c r="M15" s="13">
         <v>292</v>
       </c>
-      <c r="M14" s="15">
+      <c r="N15" s="13">
         <v>5527</v>
       </c>
-      <c r="N14" s="16">
+      <c r="O15" s="14">
         <v>18500</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E2:N2"/>
-    <mergeCell ref="E3:N3"/>
+    <mergeCell ref="E2:O2"/>
+    <mergeCell ref="E3:O3"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="E5:N6 E8:N8 E7:H7 J7:N7 E10:N14 E9:G9 I9:N9">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="E5:O15">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
+        <cfvo type="num" val="500000"/>
+        <color rgb="FFFF5651"/>
+        <color rgb="FFFFFF66"/>
         <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -1444,28 +1483,28 @@
       <c r="U5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="V5" s="7">
-        <f>LOG10(G5 + 1)</f>
+      <c r="V5" s="5">
+        <f t="shared" ref="V5:AA10" si="0">LOG10(G5 + 1)</f>
         <v>4.1801545594533485</v>
       </c>
-      <c r="W5" s="7">
-        <f>LOG10(H5 + 1)</f>
+      <c r="W5" s="5">
+        <f t="shared" si="0"/>
         <v>0.95424250943932487</v>
       </c>
-      <c r="X5" s="7">
-        <f>LOG10(I5 + 1)</f>
+      <c r="X5" s="5">
+        <f t="shared" si="0"/>
         <v>5.060323808432341</v>
       </c>
-      <c r="Y5" s="7">
-        <f>LOG10(J5 + 1)</f>
-        <v>0</v>
-      </c>
-      <c r="Z5" s="7">
-        <f>LOG10(K5 + 1)</f>
+      <c r="Y5" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z5" s="5">
+        <f t="shared" si="0"/>
         <v>3.879153246184246</v>
       </c>
-      <c r="AA5" s="7">
-        <f>LOG10(L5 + 1)</f>
+      <c r="AA5" s="5">
+        <f t="shared" si="0"/>
         <v>3.2626883443016963</v>
       </c>
     </row>
@@ -1496,28 +1535,28 @@
       <c r="U6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="V6" s="7">
-        <f>LOG10(G6 + 1)</f>
-        <v>0</v>
-      </c>
-      <c r="W6" s="7">
-        <f>LOG10(H6 + 1)</f>
+      <c r="V6" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="5">
+        <f t="shared" si="0"/>
         <v>0.90308998699194354</v>
       </c>
-      <c r="X6" s="7">
-        <f>LOG10(I6 + 1)</f>
+      <c r="X6" s="5">
+        <f t="shared" si="0"/>
         <v>0.6020599913279624</v>
       </c>
-      <c r="Y6" s="7">
-        <f>LOG10(J6 + 1)</f>
-        <v>0</v>
-      </c>
-      <c r="Z6" s="7">
-        <f>LOG10(K6 + 1)</f>
-        <v>0</v>
-      </c>
-      <c r="AA6" s="7">
-        <f>LOG10(L6 + 1)</f>
+      <c r="Y6" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="5">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1548,28 +1587,28 @@
       <c r="U7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="V7" s="7">
-        <f>LOG10(G7 + 1)</f>
+      <c r="V7" s="5">
+        <f t="shared" si="0"/>
         <v>4.3243030374868345</v>
       </c>
-      <c r="W7" s="7">
-        <f>LOG10(H7 + 1)</f>
+      <c r="W7" s="5">
+        <f t="shared" si="0"/>
         <v>5.7305893027237325</v>
       </c>
-      <c r="X7" s="7">
-        <f>LOG10(I7 + 1)</f>
+      <c r="X7" s="5">
+        <f t="shared" si="0"/>
         <v>5.4566711468721261</v>
       </c>
-      <c r="Y7" s="7">
-        <f>LOG10(J7 + 1)</f>
+      <c r="Y7" s="5">
+        <f t="shared" si="0"/>
         <v>1.7481880270062005</v>
       </c>
-      <c r="Z7" s="7">
-        <f>LOG10(K7 + 1)</f>
+      <c r="Z7" s="5">
+        <f t="shared" si="0"/>
         <v>4.0159462436575666</v>
       </c>
-      <c r="AA7" s="7">
-        <f>LOG10(L7 + 1)</f>
+      <c r="AA7" s="5">
+        <f t="shared" si="0"/>
         <v>2.7355988996981799</v>
       </c>
     </row>
@@ -1600,28 +1639,28 @@
       <c r="U8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="V8" s="7">
-        <f>LOG10(G8 + 1)</f>
+      <c r="V8" s="5">
+        <f t="shared" si="0"/>
         <v>0.90308998699194354</v>
       </c>
-      <c r="W8" s="7">
-        <f>LOG10(H8 + 1)</f>
+      <c r="W8" s="5">
+        <f t="shared" si="0"/>
         <v>3.5160062303860475</v>
       </c>
-      <c r="X8" s="7">
-        <f>LOG10(I8 + 1)</f>
+      <c r="X8" s="5">
+        <f t="shared" si="0"/>
         <v>3.1357685145678222</v>
       </c>
-      <c r="Y8" s="7">
-        <f>LOG10(J8 + 1)</f>
+      <c r="Y8" s="5">
+        <f t="shared" si="0"/>
         <v>3.643551368562945</v>
       </c>
-      <c r="Z8" s="7">
-        <f>LOG10(K8 + 1)</f>
+      <c r="Z8" s="5">
+        <f t="shared" si="0"/>
         <v>0.90308998699194354</v>
       </c>
-      <c r="AA8" s="7">
-        <f>LOG10(L8 + 1)</f>
+      <c r="AA8" s="5">
+        <f t="shared" si="0"/>
         <v>3.1495270137543478</v>
       </c>
     </row>
@@ -1652,28 +1691,28 @@
       <c r="U9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="V9" s="7">
-        <f>LOG10(G9 + 1)</f>
+      <c r="V9" s="5">
+        <f t="shared" si="0"/>
         <v>4.037864555774374</v>
       </c>
-      <c r="W9" s="7">
-        <f>LOG10(H9 + 1)</f>
-        <v>0</v>
-      </c>
-      <c r="X9" s="7">
-        <f>LOG10(I9 + 1)</f>
+      <c r="W9" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X9" s="5">
+        <f t="shared" si="0"/>
         <v>4.2143404103197346</v>
       </c>
-      <c r="Y9" s="7">
-        <f>LOG10(J9 + 1)</f>
+      <c r="Y9" s="5">
+        <f t="shared" si="0"/>
         <v>4.3444119245745467</v>
       </c>
-      <c r="Z9" s="7">
-        <f>LOG10(K9 + 1)</f>
+      <c r="Z9" s="5">
+        <f t="shared" si="0"/>
         <v>1.146128035678238</v>
       </c>
-      <c r="AA9" s="7">
-        <f>LOG10(L9 + 1)</f>
+      <c r="AA9" s="5">
+        <f t="shared" si="0"/>
         <v>4.1931524368520776</v>
       </c>
     </row>
@@ -1704,28 +1743,28 @@
       <c r="U10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="V10" s="7">
-        <f>LOG10(G10 + 1)</f>
+      <c r="V10" s="5">
+        <f t="shared" si="0"/>
         <v>3.2177470732627937</v>
       </c>
-      <c r="W10" s="7">
-        <f>LOG10(H10 + 1)</f>
-        <v>0</v>
-      </c>
-      <c r="X10" s="7">
-        <f>LOG10(I10 + 1)</f>
+      <c r="W10" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X10" s="5">
+        <f t="shared" si="0"/>
         <v>3.255272505103306</v>
       </c>
-      <c r="Y10" s="7">
-        <f>LOG10(J10 + 1)</f>
+      <c r="Y10" s="5">
+        <f t="shared" si="0"/>
         <v>0.77815125038364363</v>
       </c>
-      <c r="Z10" s="7">
-        <f>LOG10(K10 + 1)</f>
+      <c r="Z10" s="5">
+        <f t="shared" si="0"/>
         <v>0.84509804001425681</v>
       </c>
-      <c r="AA10" s="7">
-        <f>LOG10(L10 + 1)</f>
+      <c r="AA10" s="5">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>